<commit_message>
2.0 Gestor de fichas
</commit_message>
<xml_diff>
--- a/data/propuestas_artisticas.xlsx
+++ b/data/propuestas_artisticas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7430" uniqueCount="2417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7744" uniqueCount="2423">
   <si>
     <t>Edad</t>
   </si>
@@ -7278,6 +7278,24 @@
   </si>
   <si>
     <t>P313</t>
+  </si>
+  <si>
+    <t>Ficha</t>
+  </si>
+  <si>
+    <t>MAPALE</t>
+  </si>
+  <si>
+    <t>SON_NEGRO</t>
+  </si>
+  <si>
+    <t>COMPARSA_FANT</t>
+  </si>
+  <si>
+    <t>COMPARSA_TRAD</t>
+  </si>
+  <si>
+    <t>DANZAS_ESP</t>
   </si>
 </sst>
 </file>
@@ -7329,7 +7347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -7395,11 +7413,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7435,6 +7473,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7728,18 +7775,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE314"/>
+  <dimension ref="A1:AF314"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B314"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="26" max="26" width="36.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="50" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:32" ht="50" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2086</v>
       </c>
@@ -7833,8 +7881,11 @@
       <c r="AE1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="AF1" s="13" t="s">
+        <v>2417</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>2026</v>
       </c>
@@ -7928,8 +7979,11 @@
       <c r="AE2" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF2" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2026</v>
       </c>
@@ -8023,8 +8077,11 @@
       <c r="AE3" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF3" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2026</v>
       </c>
@@ -8118,8 +8175,11 @@
       <c r="AE4" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF4" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>2026</v>
       </c>
@@ -8213,8 +8273,11 @@
       <c r="AE5" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF5" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>2026</v>
       </c>
@@ -8308,8 +8371,11 @@
       <c r="AE6" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF6" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>2026</v>
       </c>
@@ -8403,8 +8469,11 @@
       <c r="AE7" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF7" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>2026</v>
       </c>
@@ -8498,8 +8567,11 @@
       <c r="AE8" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF8" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>2026</v>
       </c>
@@ -8593,8 +8665,11 @@
       <c r="AE9" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF9" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>2026</v>
       </c>
@@ -8688,8 +8763,11 @@
       <c r="AE10" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF10" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>2026</v>
       </c>
@@ -8783,8 +8861,11 @@
       <c r="AE11" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF11" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="12" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>2026</v>
       </c>
@@ -8878,8 +8959,11 @@
       <c r="AE12" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF12" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>2026</v>
       </c>
@@ -8973,8 +9057,11 @@
       <c r="AE13" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF13" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>2026</v>
       </c>
@@ -9068,8 +9155,11 @@
       <c r="AE14" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF14" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="15" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>2026</v>
       </c>
@@ -9163,8 +9253,11 @@
       <c r="AE15" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF15" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="16" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>2026</v>
       </c>
@@ -9258,8 +9351,11 @@
       <c r="AE16" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF16" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="17" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>2026</v>
       </c>
@@ -9353,8 +9449,11 @@
       <c r="AE17" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF17" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="18" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>2026</v>
       </c>
@@ -9448,8 +9547,11 @@
       <c r="AE18" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF18" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>2026</v>
       </c>
@@ -9543,8 +9645,11 @@
       <c r="AE19" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF19" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>2026</v>
       </c>
@@ -9638,8 +9743,11 @@
       <c r="AE20" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF20" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="21" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>2026</v>
       </c>
@@ -9733,8 +9841,11 @@
       <c r="AE21" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF21" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="22" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>2026</v>
       </c>
@@ -9828,8 +9939,11 @@
       <c r="AE22" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF22" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="23" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>2026</v>
       </c>
@@ -9923,8 +10037,11 @@
       <c r="AE23" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF23" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>2026</v>
       </c>
@@ -10018,8 +10135,11 @@
       <c r="AE24" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF24" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>2026</v>
       </c>
@@ -10113,8 +10233,11 @@
       <c r="AE25" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF25" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="26" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>2026</v>
       </c>
@@ -10208,8 +10331,11 @@
       <c r="AE26" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF26" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>2026</v>
       </c>
@@ -10303,8 +10429,11 @@
       <c r="AE27" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF27" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>2026</v>
       </c>
@@ -10398,8 +10527,11 @@
       <c r="AE28" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF28" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="29" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>2026</v>
       </c>
@@ -10493,8 +10625,11 @@
       <c r="AE29" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF29" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="30" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>2026</v>
       </c>
@@ -10588,8 +10723,11 @@
       <c r="AE30" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF30" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="31" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>2026</v>
       </c>
@@ -10683,8 +10821,11 @@
       <c r="AE31" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF31" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>2026</v>
       </c>
@@ -10778,8 +10919,11 @@
       <c r="AE32" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF32" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="33" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>2026</v>
       </c>
@@ -10873,8 +11017,11 @@
       <c r="AE33" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF33" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="34" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>2026</v>
       </c>
@@ -10968,8 +11115,11 @@
       <c r="AE34" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF34" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="35" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>2026</v>
       </c>
@@ -11063,8 +11213,11 @@
       <c r="AE35" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF35" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="36" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>2026</v>
       </c>
@@ -11158,8 +11311,11 @@
       <c r="AE36" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF36" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="37" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>2026</v>
       </c>
@@ -11253,8 +11409,11 @@
       <c r="AE37" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF37" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="38" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>2026</v>
       </c>
@@ -11348,8 +11507,11 @@
       <c r="AE38" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF38" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="39" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>2026</v>
       </c>
@@ -11443,8 +11605,11 @@
       <c r="AE39" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF39" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="40" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>2026</v>
       </c>
@@ -11538,8 +11703,11 @@
       <c r="AE40" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF40" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="41" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>2026</v>
       </c>
@@ -11633,8 +11801,11 @@
       <c r="AE41" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF41" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="42" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>2026</v>
       </c>
@@ -11728,8 +11899,11 @@
       <c r="AE42" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF42" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="43" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>2026</v>
       </c>
@@ -11823,8 +11997,11 @@
       <c r="AE43" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF43" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="44" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>2026</v>
       </c>
@@ -11918,8 +12095,11 @@
       <c r="AE44" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF44" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="45" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>2026</v>
       </c>
@@ -12013,8 +12193,11 @@
       <c r="AE45" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF45" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="46" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>2026</v>
       </c>
@@ -12108,8 +12291,11 @@
       <c r="AE46" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF46" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="47" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>2026</v>
       </c>
@@ -12203,8 +12389,11 @@
       <c r="AE47" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF47" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="48" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>2026</v>
       </c>
@@ -12298,8 +12487,11 @@
       <c r="AE48" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF48" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="49" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>2026</v>
       </c>
@@ -12393,8 +12585,11 @@
       <c r="AE49" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF49" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="50" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>2026</v>
       </c>
@@ -12488,8 +12683,11 @@
       <c r="AE50" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF50" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="51" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>2026</v>
       </c>
@@ -12583,8 +12781,11 @@
       <c r="AE51" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF51" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="52" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>2026</v>
       </c>
@@ -12678,8 +12879,11 @@
       <c r="AE52" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF52" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="53" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>2026</v>
       </c>
@@ -12773,8 +12977,11 @@
       <c r="AE53" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF53" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="54" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>2026</v>
       </c>
@@ -12868,8 +13075,11 @@
       <c r="AE54" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF54" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="55" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>2026</v>
       </c>
@@ -12963,8 +13173,11 @@
       <c r="AE55" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF55" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="56" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>2026</v>
       </c>
@@ -13058,8 +13271,11 @@
       <c r="AE56" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF56" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="57" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>2026</v>
       </c>
@@ -13153,8 +13369,11 @@
       <c r="AE57" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF57" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="58" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>2026</v>
       </c>
@@ -13248,8 +13467,11 @@
       <c r="AE58" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF58" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="59" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>2026</v>
       </c>
@@ -13343,8 +13565,11 @@
       <c r="AE59" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF59" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="60" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>2026</v>
       </c>
@@ -13438,8 +13663,11 @@
       <c r="AE60" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF60" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="61" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>2026</v>
       </c>
@@ -13533,8 +13761,11 @@
       <c r="AE61" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF61" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="62" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>2026</v>
       </c>
@@ -13628,8 +13859,11 @@
       <c r="AE62" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF62" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="63" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>2026</v>
       </c>
@@ -13723,8 +13957,11 @@
       <c r="AE63" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF63" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="64" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>2026</v>
       </c>
@@ -13818,8 +14055,11 @@
       <c r="AE64" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF64" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="65" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
         <v>2026</v>
       </c>
@@ -13913,8 +14153,11 @@
       <c r="AE65" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF65" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="66" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>2026</v>
       </c>
@@ -14008,8 +14251,11 @@
       <c r="AE66" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF66" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="67" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>2026</v>
       </c>
@@ -14103,8 +14349,11 @@
       <c r="AE67" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF67" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="68" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>2026</v>
       </c>
@@ -14198,8 +14447,11 @@
       <c r="AE68" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF68" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="69" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
         <v>2026</v>
       </c>
@@ -14293,8 +14545,11 @@
       <c r="AE69" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF69" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="70" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
         <v>2026</v>
       </c>
@@ -14388,8 +14643,11 @@
       <c r="AE70" s="6" t="s">
         <v>493</v>
       </c>
+      <c r="AF70" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="71" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
         <v>2026</v>
       </c>
@@ -14483,8 +14741,11 @@
       <c r="AE71" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF71" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="72" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
         <v>2026</v>
       </c>
@@ -14578,8 +14839,11 @@
       <c r="AE72" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="AF72" s="14" t="s">
+        <v>2422</v>
+      </c>
     </row>
-    <row r="73" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
         <v>2026</v>
       </c>
@@ -14673,8 +14937,11 @@
       <c r="AE73" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF73" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="74" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
         <v>2026</v>
       </c>
@@ -14768,8 +15035,11 @@
       <c r="AE74" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF74" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="75" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
         <v>2026</v>
       </c>
@@ -14863,8 +15133,11 @@
       <c r="AE75" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF75" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="76" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
         <v>2026</v>
       </c>
@@ -14958,8 +15231,11 @@
       <c r="AE76" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF76" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="77" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
         <v>2026</v>
       </c>
@@ -15053,8 +15329,11 @@
       <c r="AE77" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF77" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="78" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
         <v>2026</v>
       </c>
@@ -15148,8 +15427,11 @@
       <c r="AE78" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF78" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="79" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
         <v>2026</v>
       </c>
@@ -15243,8 +15525,11 @@
       <c r="AE79" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF79" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="80" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
         <v>2026</v>
       </c>
@@ -15338,8 +15623,11 @@
       <c r="AE80" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF80" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="81" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
         <v>2026</v>
       </c>
@@ -15433,8 +15721,11 @@
       <c r="AE81" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF81" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="82" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
         <v>2026</v>
       </c>
@@ -15528,8 +15819,11 @@
       <c r="AE82" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF82" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="83" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
         <v>2026</v>
       </c>
@@ -15623,8 +15917,11 @@
       <c r="AE83" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF83" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="84" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
         <v>2026</v>
       </c>
@@ -15718,8 +16015,11 @@
       <c r="AE84" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF84" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="85" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
         <v>2026</v>
       </c>
@@ -15813,8 +16113,11 @@
       <c r="AE85" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF85" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="86" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
         <v>2026</v>
       </c>
@@ -15908,8 +16211,11 @@
       <c r="AE86" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF86" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="87" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
         <v>2026</v>
       </c>
@@ -16003,8 +16309,11 @@
       <c r="AE87" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF87" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="88" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
         <v>2026</v>
       </c>
@@ -16098,8 +16407,11 @@
       <c r="AE88" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF88" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="89" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
         <v>2026</v>
       </c>
@@ -16193,8 +16505,11 @@
       <c r="AE89" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF89" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="90" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
         <v>2026</v>
       </c>
@@ -16288,8 +16603,11 @@
       <c r="AE90" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF90" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="91" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
         <v>2026</v>
       </c>
@@ -16383,8 +16701,11 @@
       <c r="AE91" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF91" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="92" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
         <v>2026</v>
       </c>
@@ -16478,8 +16799,11 @@
       <c r="AE92" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF92" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="93" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
         <v>2026</v>
       </c>
@@ -16573,8 +16897,11 @@
       <c r="AE93" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF93" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="94" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
         <v>2026</v>
       </c>
@@ -16668,8 +16995,11 @@
       <c r="AE94" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF94" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="95" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
         <v>2026</v>
       </c>
@@ -16763,8 +17093,11 @@
       <c r="AE95" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF95" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="96" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
         <v>2026</v>
       </c>
@@ -16858,8 +17191,11 @@
       <c r="AE96" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF96" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="97" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
         <v>2026</v>
       </c>
@@ -16953,8 +17289,11 @@
       <c r="AE97" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF97" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="98" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
         <v>2026</v>
       </c>
@@ -17048,8 +17387,11 @@
       <c r="AE98" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF98" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="99" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
         <v>2026</v>
       </c>
@@ -17143,8 +17485,11 @@
       <c r="AE99" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF99" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="100" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
         <v>2026</v>
       </c>
@@ -17238,8 +17583,11 @@
       <c r="AE100" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF100" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="101" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
         <v>2026</v>
       </c>
@@ -17333,8 +17681,11 @@
       <c r="AE101" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF101" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="102" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
         <v>2026</v>
       </c>
@@ -17428,8 +17779,11 @@
       <c r="AE102" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF102" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="103" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
         <v>2026</v>
       </c>
@@ -17523,8 +17877,11 @@
       <c r="AE103" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF103" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="104" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
         <v>2026</v>
       </c>
@@ -17618,8 +17975,11 @@
       <c r="AE104" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF104" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="105" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
         <v>2026</v>
       </c>
@@ -17713,8 +18073,11 @@
       <c r="AE105" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF105" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="106" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
         <v>2026</v>
       </c>
@@ -17808,8 +18171,11 @@
       <c r="AE106" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF106" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="107" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
         <v>2026</v>
       </c>
@@ -17903,8 +18269,11 @@
       <c r="AE107" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF107" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="108" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
         <v>2026</v>
       </c>
@@ -17998,8 +18367,11 @@
       <c r="AE108" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF108" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="109" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A109" s="6">
         <v>2026</v>
       </c>
@@ -18093,8 +18465,11 @@
       <c r="AE109" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF109" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="110" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A110" s="6">
         <v>2026</v>
       </c>
@@ -18188,8 +18563,11 @@
       <c r="AE110" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF110" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="111" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A111" s="6">
         <v>2026</v>
       </c>
@@ -18283,8 +18661,11 @@
       <c r="AE111" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF111" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="112" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A112" s="6">
         <v>2026</v>
       </c>
@@ -18378,8 +18759,11 @@
       <c r="AE112" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF112" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="113" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A113" s="6">
         <v>2026</v>
       </c>
@@ -18473,8 +18857,11 @@
       <c r="AE113" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF113" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="114" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A114" s="6">
         <v>2026</v>
       </c>
@@ -18568,8 +18955,11 @@
       <c r="AE114" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF114" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="115" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A115" s="6">
         <v>2026</v>
       </c>
@@ -18663,8 +19053,11 @@
       <c r="AE115" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF115" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="116" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A116" s="6">
         <v>2026</v>
       </c>
@@ -18758,8 +19151,11 @@
       <c r="AE116" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF116" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="117" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A117" s="6">
         <v>2026</v>
       </c>
@@ -18853,8 +19249,11 @@
       <c r="AE117" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF117" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="118" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A118" s="6">
         <v>2026</v>
       </c>
@@ -18948,8 +19347,11 @@
       <c r="AE118" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF118" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="119" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A119" s="6">
         <v>2026</v>
       </c>
@@ -19043,8 +19445,11 @@
       <c r="AE119" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF119" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="120" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A120" s="6">
         <v>2026</v>
       </c>
@@ -19138,8 +19543,11 @@
       <c r="AE120" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF120" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="121" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A121" s="6">
         <v>2026</v>
       </c>
@@ -19233,8 +19641,11 @@
       <c r="AE121" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF121" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="122" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A122" s="6">
         <v>2026</v>
       </c>
@@ -19328,8 +19739,11 @@
       <c r="AE122" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF122" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="123" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A123" s="6">
         <v>2026</v>
       </c>
@@ -19423,8 +19837,11 @@
       <c r="AE123" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF123" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="124" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A124" s="6">
         <v>2026</v>
       </c>
@@ -19518,8 +19935,11 @@
       <c r="AE124" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF124" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="125" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A125" s="6">
         <v>2026</v>
       </c>
@@ -19613,8 +20033,11 @@
       <c r="AE125" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF125" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="126" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A126" s="6">
         <v>2026</v>
       </c>
@@ -19708,8 +20131,11 @@
       <c r="AE126" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF126" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="127" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A127" s="6">
         <v>2026</v>
       </c>
@@ -19803,8 +20229,11 @@
       <c r="AE127" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF127" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="128" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A128" s="6">
         <v>2026</v>
       </c>
@@ -19898,8 +20327,11 @@
       <c r="AE128" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF128" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="129" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A129" s="6">
         <v>2026</v>
       </c>
@@ -19993,8 +20425,11 @@
       <c r="AE129" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF129" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="130" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A130" s="6">
         <v>2026</v>
       </c>
@@ -20088,8 +20523,11 @@
       <c r="AE130" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF130" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="131" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A131" s="6">
         <v>2026</v>
       </c>
@@ -20183,8 +20621,11 @@
       <c r="AE131" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF131" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="132" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A132" s="6">
         <v>2026</v>
       </c>
@@ -20278,8 +20719,11 @@
       <c r="AE132" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF132" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="133" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A133" s="6">
         <v>2026</v>
       </c>
@@ -20373,8 +20817,11 @@
       <c r="AE133" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF133" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="134" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A134" s="6">
         <v>2026</v>
       </c>
@@ -20468,8 +20915,11 @@
       <c r="AE134" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF134" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="135" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A135" s="6">
         <v>2026</v>
       </c>
@@ -20563,8 +21013,11 @@
       <c r="AE135" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF135" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="136" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A136" s="6">
         <v>2026</v>
       </c>
@@ -20658,8 +21111,11 @@
       <c r="AE136" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF136" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="137" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A137" s="6">
         <v>2026</v>
       </c>
@@ -20753,8 +21209,11 @@
       <c r="AE137" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF137" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="138" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A138" s="6">
         <v>2026</v>
       </c>
@@ -20848,8 +21307,11 @@
       <c r="AE138" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF138" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="139" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A139" s="6">
         <v>2026</v>
       </c>
@@ -20943,8 +21405,11 @@
       <c r="AE139" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF139" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="140" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A140" s="6">
         <v>2026</v>
       </c>
@@ -21038,8 +21503,11 @@
       <c r="AE140" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF140" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="141" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
         <v>2026</v>
       </c>
@@ -21133,8 +21601,11 @@
       <c r="AE141" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF141" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="142" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A142" s="6">
         <v>2026</v>
       </c>
@@ -21228,8 +21699,11 @@
       <c r="AE142" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF142" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="143" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A143" s="6">
         <v>2026</v>
       </c>
@@ -21323,8 +21797,11 @@
       <c r="AE143" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF143" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="144" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A144" s="6">
         <v>2026</v>
       </c>
@@ -21418,8 +21895,11 @@
       <c r="AE144" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF144" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="145" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A145" s="6">
         <v>2026</v>
       </c>
@@ -21513,8 +21993,11 @@
       <c r="AE145" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF145" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="146" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A146" s="6">
         <v>2026</v>
       </c>
@@ -21608,8 +22091,11 @@
       <c r="AE146" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF146" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="147" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A147" s="6">
         <v>2026</v>
       </c>
@@ -21703,8 +22189,11 @@
       <c r="AE147" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF147" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="148" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A148" s="6">
         <v>2026</v>
       </c>
@@ -21798,8 +22287,11 @@
       <c r="AE148" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF148" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="149" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A149" s="6">
         <v>2026</v>
       </c>
@@ -21893,8 +22385,11 @@
       <c r="AE149" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF149" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="150" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A150" s="6">
         <v>2026</v>
       </c>
@@ -21988,8 +22483,11 @@
       <c r="AE150" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF150" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="151" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A151" s="6">
         <v>2026</v>
       </c>
@@ -22083,8 +22581,11 @@
       <c r="AE151" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF151" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="152" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A152" s="6">
         <v>2026</v>
       </c>
@@ -22178,8 +22679,11 @@
       <c r="AE152" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF152" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="153" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A153" s="6">
         <v>2026</v>
       </c>
@@ -22273,8 +22777,11 @@
       <c r="AE153" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF153" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="154" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A154" s="6">
         <v>2026</v>
       </c>
@@ -22368,8 +22875,11 @@
       <c r="AE154" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF154" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="155" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A155" s="6">
         <v>2026</v>
       </c>
@@ -22463,8 +22973,11 @@
       <c r="AE155" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF155" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="156" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A156" s="6">
         <v>2026</v>
       </c>
@@ -22558,8 +23071,11 @@
       <c r="AE156" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF156" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="157" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A157" s="6">
         <v>2026</v>
       </c>
@@ -22653,8 +23169,11 @@
       <c r="AE157" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF157" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="158" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A158" s="6">
         <v>2026</v>
       </c>
@@ -22748,8 +23267,11 @@
       <c r="AE158" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF158" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="159" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A159" s="6">
         <v>2026</v>
       </c>
@@ -22843,8 +23365,11 @@
       <c r="AE159" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF159" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="160" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A160" s="6">
         <v>2026</v>
       </c>
@@ -22938,8 +23463,11 @@
       <c r="AE160" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF160" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="161" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A161" s="6">
         <v>2026</v>
       </c>
@@ -23033,8 +23561,11 @@
       <c r="AE161" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF161" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="162" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A162" s="6">
         <v>2026</v>
       </c>
@@ -23128,8 +23659,11 @@
       <c r="AE162" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF162" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="163" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A163" s="6">
         <v>2026</v>
       </c>
@@ -23223,8 +23757,11 @@
       <c r="AE163" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF163" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="164" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A164" s="6">
         <v>2026</v>
       </c>
@@ -23318,8 +23855,11 @@
       <c r="AE164" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF164" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="165" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A165" s="6">
         <v>2026</v>
       </c>
@@ -23413,8 +23953,11 @@
       <c r="AE165" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF165" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="166" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A166" s="6">
         <v>2026</v>
       </c>
@@ -23508,8 +24051,11 @@
       <c r="AE166" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF166" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="167" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A167" s="6">
         <v>2026</v>
       </c>
@@ -23603,8 +24149,11 @@
       <c r="AE167" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF167" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="168" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A168" s="6">
         <v>2026</v>
       </c>
@@ -23698,8 +24247,11 @@
       <c r="AE168" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF168" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="169" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A169" s="6">
         <v>2026</v>
       </c>
@@ -23793,8 +24345,11 @@
       <c r="AE169" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF169" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="170" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A170" s="6">
         <v>2026</v>
       </c>
@@ -23888,8 +24443,11 @@
       <c r="AE170" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF170" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="171" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A171" s="6">
         <v>2026</v>
       </c>
@@ -23983,8 +24541,11 @@
       <c r="AE171" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF171" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="172" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A172" s="6">
         <v>2026</v>
       </c>
@@ -24078,8 +24639,11 @@
       <c r="AE172" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF172" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="173" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A173" s="6">
         <v>2026</v>
       </c>
@@ -24173,8 +24737,11 @@
       <c r="AE173" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF173" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="174" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A174" s="6">
         <v>2026</v>
       </c>
@@ -24268,8 +24835,11 @@
       <c r="AE174" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF174" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="175" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A175" s="6">
         <v>2026</v>
       </c>
@@ -24363,8 +24933,11 @@
       <c r="AE175" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF175" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="176" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A176" s="6">
         <v>2026</v>
       </c>
@@ -24458,8 +25031,11 @@
       <c r="AE176" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF176" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="177" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A177" s="6">
         <v>2026</v>
       </c>
@@ -24553,8 +25129,11 @@
       <c r="AE177" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF177" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="178" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A178" s="6">
         <v>2026</v>
       </c>
@@ -24648,8 +25227,11 @@
       <c r="AE178" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF178" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="179" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A179" s="6">
         <v>2026</v>
       </c>
@@ -24743,8 +25325,11 @@
       <c r="AE179" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="AF179" s="14" t="s">
+        <v>2421</v>
+      </c>
     </row>
-    <row r="180" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A180" s="6">
         <v>2026</v>
       </c>
@@ -24838,8 +25423,11 @@
       <c r="AE180" s="6" t="s">
         <v>463</v>
       </c>
+      <c r="AF180" s="14" t="s">
+        <v>2420</v>
+      </c>
     </row>
-    <row r="181" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A181" s="6">
         <v>2026</v>
       </c>
@@ -24933,8 +25521,11 @@
       <c r="AE181" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF181" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="182" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A182" s="9">
         <v>2026</v>
       </c>
@@ -25028,8 +25619,11 @@
       <c r="AE182" s="9" t="s">
         <v>33</v>
       </c>
+      <c r="AF182" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="183" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A183" s="6">
         <v>2026</v>
       </c>
@@ -25123,8 +25717,11 @@
       <c r="AE183" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF183" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="184" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A184" s="6">
         <v>2026</v>
       </c>
@@ -25218,8 +25815,11 @@
       <c r="AE184" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF184" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="185" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A185" s="6">
         <v>2026</v>
       </c>
@@ -25313,8 +25913,11 @@
       <c r="AE185" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF185" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="186" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A186" s="6">
         <v>2026</v>
       </c>
@@ -25408,8 +26011,11 @@
       <c r="AE186" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF186" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="187" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A187" s="6">
         <v>2026</v>
       </c>
@@ -25503,8 +26109,11 @@
       <c r="AE187" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF187" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="188" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A188" s="6">
         <v>2026</v>
       </c>
@@ -25598,8 +26207,11 @@
       <c r="AE188" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF188" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="189" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A189" s="6">
         <v>2026</v>
       </c>
@@ -25693,8 +26305,11 @@
       <c r="AE189" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF189" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="190" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A190" s="6">
         <v>2026</v>
       </c>
@@ -25788,8 +26403,11 @@
       <c r="AE190" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF190" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="191" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A191" s="6">
         <v>2026</v>
       </c>
@@ -25883,8 +26501,11 @@
       <c r="AE191" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF191" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="192" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A192" s="6">
         <v>2026</v>
       </c>
@@ -25978,8 +26599,11 @@
       <c r="AE192" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF192" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="193" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A193" s="6">
         <v>2026</v>
       </c>
@@ -26073,8 +26697,11 @@
       <c r="AE193" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF193" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="194" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A194" s="6">
         <v>2026</v>
       </c>
@@ -26168,8 +26795,11 @@
       <c r="AE194" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF194" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="195" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A195" s="6">
         <v>2026</v>
       </c>
@@ -26263,8 +26893,11 @@
       <c r="AE195" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF195" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="196" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A196" s="6">
         <v>2026</v>
       </c>
@@ -26358,8 +26991,11 @@
       <c r="AE196" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF196" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="197" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A197" s="6">
         <v>2026</v>
       </c>
@@ -26453,8 +27089,11 @@
       <c r="AE197" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF197" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="198" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A198" s="6">
         <v>2026</v>
       </c>
@@ -26548,8 +27187,11 @@
       <c r="AE198" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF198" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="199" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A199" s="6">
         <v>2026</v>
       </c>
@@ -26643,8 +27285,11 @@
       <c r="AE199" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF199" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="200" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A200" s="6">
         <v>2026</v>
       </c>
@@ -26738,8 +27383,11 @@
       <c r="AE200" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF200" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="201" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A201" s="6">
         <v>2026</v>
       </c>
@@ -26833,8 +27481,11 @@
       <c r="AE201" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF201" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="202" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A202" s="6">
         <v>2026</v>
       </c>
@@ -26928,8 +27579,11 @@
       <c r="AE202" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF202" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="203" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A203" s="6">
         <v>2026</v>
       </c>
@@ -27023,8 +27677,11 @@
       <c r="AE203" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF203" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="204" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A204" s="6">
         <v>2026</v>
       </c>
@@ -27118,8 +27775,11 @@
       <c r="AE204" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF204" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="205" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A205" s="6">
         <v>2026</v>
       </c>
@@ -27213,8 +27873,11 @@
       <c r="AE205" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF205" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="206" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A206" s="6">
         <v>2026</v>
       </c>
@@ -27308,8 +27971,11 @@
       <c r="AE206" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF206" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="207" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A207" s="6">
         <v>2026</v>
       </c>
@@ -27403,8 +28069,11 @@
       <c r="AE207" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF207" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="208" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A208" s="6">
         <v>2026</v>
       </c>
@@ -27498,8 +28167,11 @@
       <c r="AE208" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF208" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="209" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A209" s="6">
         <v>2026</v>
       </c>
@@ -27593,8 +28265,11 @@
       <c r="AE209" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF209" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="210" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A210" s="6">
         <v>2026</v>
       </c>
@@ -27688,8 +28363,11 @@
       <c r="AE210" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF210" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="211" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A211" s="6">
         <v>2026</v>
       </c>
@@ -27783,8 +28461,11 @@
       <c r="AE211" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF211" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="212" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A212" s="6">
         <v>2026</v>
       </c>
@@ -27878,8 +28559,11 @@
       <c r="AE212" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF212" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="213" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A213" s="6">
         <v>2026</v>
       </c>
@@ -27973,8 +28657,11 @@
       <c r="AE213" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF213" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="214" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A214" s="6">
         <v>2026</v>
       </c>
@@ -28068,8 +28755,11 @@
       <c r="AE214" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF214" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="215" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A215" s="6">
         <v>2026</v>
       </c>
@@ -28163,8 +28853,11 @@
       <c r="AE215" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF215" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="216" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A216" s="6">
         <v>2026</v>
       </c>
@@ -28258,8 +28951,11 @@
       <c r="AE216" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF216" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="217" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A217" s="6">
         <v>2026</v>
       </c>
@@ -28353,8 +29049,11 @@
       <c r="AE217" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF217" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="218" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A218" s="6">
         <v>2026</v>
       </c>
@@ -28448,8 +29147,11 @@
       <c r="AE218" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF218" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="219" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A219" s="6">
         <v>2026</v>
       </c>
@@ -28543,8 +29245,11 @@
       <c r="AE219" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF219" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="220" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A220" s="6">
         <v>2026</v>
       </c>
@@ -28638,8 +29343,11 @@
       <c r="AE220" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF220" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="221" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A221" s="6">
         <v>2026</v>
       </c>
@@ -28733,8 +29441,11 @@
       <c r="AE221" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF221" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="222" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A222" s="6">
         <v>2026</v>
       </c>
@@ -28828,8 +29539,11 @@
       <c r="AE222" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF222" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="223" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A223" s="6">
         <v>2026</v>
       </c>
@@ -28923,8 +29637,11 @@
       <c r="AE223" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF223" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="224" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A224" s="6">
         <v>2026</v>
       </c>
@@ -29018,8 +29735,11 @@
       <c r="AE224" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF224" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="225" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A225" s="6">
         <v>2026</v>
       </c>
@@ -29113,8 +29833,11 @@
       <c r="AE225" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF225" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="226" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A226" s="6">
         <v>2026</v>
       </c>
@@ -29208,8 +29931,11 @@
       <c r="AE226" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF226" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="227" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A227" s="6">
         <v>2026</v>
       </c>
@@ -29303,8 +30029,11 @@
       <c r="AE227" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF227" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="228" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A228" s="6">
         <v>2026</v>
       </c>
@@ -29398,8 +30127,11 @@
       <c r="AE228" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF228" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="229" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A229" s="6">
         <v>2026</v>
       </c>
@@ -29493,8 +30225,11 @@
       <c r="AE229" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="AF229" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="230" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A230" s="6">
         <v>2026</v>
       </c>
@@ -29588,8 +30323,11 @@
       <c r="AE230" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF230" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="231" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A231" s="6">
         <v>2026</v>
       </c>
@@ -29683,8 +30421,11 @@
       <c r="AE231" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF231" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="232" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A232" s="6">
         <v>2026</v>
       </c>
@@ -29778,8 +30519,11 @@
       <c r="AE232" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF232" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="233" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A233" s="6">
         <v>2026</v>
       </c>
@@ -29873,8 +30617,11 @@
       <c r="AE233" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF233" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="234" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A234" s="6">
         <v>2026</v>
       </c>
@@ -29968,8 +30715,11 @@
       <c r="AE234" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF234" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="235" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A235" s="6">
         <v>2026</v>
       </c>
@@ -30063,8 +30813,11 @@
       <c r="AE235" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF235" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="236" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A236" s="6">
         <v>2026</v>
       </c>
@@ -30158,8 +30911,11 @@
       <c r="AE236" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF236" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="237" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A237" s="6">
         <v>2026</v>
       </c>
@@ -30253,8 +31009,11 @@
       <c r="AE237" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF237" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="238" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A238" s="6">
         <v>2026</v>
       </c>
@@ -30348,8 +31107,11 @@
       <c r="AE238" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF238" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="239" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A239" s="6">
         <v>2026</v>
       </c>
@@ -30443,8 +31205,11 @@
       <c r="AE239" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF239" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="240" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A240" s="6">
         <v>2026</v>
       </c>
@@ -30538,8 +31303,11 @@
       <c r="AE240" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF240" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="241" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A241" s="6">
         <v>2026</v>
       </c>
@@ -30633,8 +31401,11 @@
       <c r="AE241" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF241" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="242" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A242" s="6">
         <v>2026</v>
       </c>
@@ -30728,8 +31499,11 @@
       <c r="AE242" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF242" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="243" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A243" s="6">
         <v>2026</v>
       </c>
@@ -30823,8 +31597,11 @@
       <c r="AE243" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF243" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="244" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A244" s="6">
         <v>2026</v>
       </c>
@@ -30918,8 +31695,11 @@
       <c r="AE244" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF244" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="245" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A245" s="6">
         <v>2026</v>
       </c>
@@ -31013,8 +31793,11 @@
       <c r="AE245" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF245" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="246" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A246" s="6">
         <v>2026</v>
       </c>
@@ -31108,8 +31891,11 @@
       <c r="AE246" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF246" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="247" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A247" s="6">
         <v>2026</v>
       </c>
@@ -31203,8 +31989,11 @@
       <c r="AE247" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF247" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="248" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A248" s="6">
         <v>2026</v>
       </c>
@@ -31298,8 +32087,11 @@
       <c r="AE248" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF248" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="249" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A249" s="6">
         <v>2026</v>
       </c>
@@ -31393,8 +32185,11 @@
       <c r="AE249" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF249" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="250" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A250" s="6">
         <v>2026</v>
       </c>
@@ -31488,8 +32283,11 @@
       <c r="AE250" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF250" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="251" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A251" s="6">
         <v>2026</v>
       </c>
@@ -31581,8 +32379,11 @@
         <v>33</v>
       </c>
       <c r="AE251" s="6"/>
+      <c r="AF251" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="252" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A252" s="6">
         <v>2026</v>
       </c>
@@ -31676,8 +32477,11 @@
       <c r="AE252" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF252" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="253" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A253" s="6">
         <v>2026</v>
       </c>
@@ -31771,8 +32575,11 @@
       <c r="AE253" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF253" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="254" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A254" s="6">
         <v>2026</v>
       </c>
@@ -31866,8 +32673,11 @@
       <c r="AE254" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF254" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="255" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A255" s="6">
         <v>2026</v>
       </c>
@@ -31961,8 +32771,11 @@
       <c r="AE255" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF255" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="256" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A256" s="6">
         <v>2026</v>
       </c>
@@ -32056,8 +32869,11 @@
       <c r="AE256" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF256" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="257" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A257" s="6">
         <v>2026</v>
       </c>
@@ -32151,8 +32967,11 @@
       <c r="AE257" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF257" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="258" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A258" s="6">
         <v>2026</v>
       </c>
@@ -32246,8 +33065,11 @@
       <c r="AE258" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF258" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="259" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A259" s="6">
         <v>2026</v>
       </c>
@@ -32341,8 +33163,11 @@
       <c r="AE259" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF259" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="260" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A260" s="6">
         <v>2026</v>
       </c>
@@ -32436,8 +33261,11 @@
       <c r="AE260" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF260" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="261" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A261" s="6">
         <v>2026</v>
       </c>
@@ -32531,8 +33359,11 @@
       <c r="AE261" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF261" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="262" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A262" s="6">
         <v>2026</v>
       </c>
@@ -32626,8 +33457,11 @@
       <c r="AE262" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF262" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="263" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A263" s="6">
         <v>2026</v>
       </c>
@@ -32721,8 +33555,11 @@
       <c r="AE263" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF263" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="264" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A264" s="6">
         <v>2026</v>
       </c>
@@ -32816,8 +33653,11 @@
       <c r="AE264" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF264" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="265" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A265" s="6">
         <v>2026</v>
       </c>
@@ -32911,8 +33751,11 @@
       <c r="AE265" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF265" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="266" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A266" s="6">
         <v>2026</v>
       </c>
@@ -33006,8 +33849,11 @@
       <c r="AE266" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF266" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="267" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A267" s="6">
         <v>2026</v>
       </c>
@@ -33101,8 +33947,11 @@
       <c r="AE267" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF267" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="268" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A268" s="6">
         <v>2026</v>
       </c>
@@ -33196,8 +34045,11 @@
       <c r="AE268" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF268" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="269" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A269" s="6">
         <v>2026</v>
       </c>
@@ -33291,8 +34143,11 @@
       <c r="AE269" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF269" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="270" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A270" s="6">
         <v>2026</v>
       </c>
@@ -33386,8 +34241,11 @@
       <c r="AE270" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF270" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="271" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A271" s="6">
         <v>2026</v>
       </c>
@@ -33481,8 +34339,11 @@
       <c r="AE271" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF271" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="272" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A272" s="6">
         <v>2026</v>
       </c>
@@ -33576,8 +34437,11 @@
       <c r="AE272" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF272" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="273" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A273" s="6">
         <v>2026</v>
       </c>
@@ -33671,8 +34535,11 @@
       <c r="AE273" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF273" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="274" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A274" s="6">
         <v>2026</v>
       </c>
@@ -33766,8 +34633,11 @@
       <c r="AE274" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF274" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="275" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A275" s="6">
         <v>2026</v>
       </c>
@@ -33861,8 +34731,11 @@
       <c r="AE275" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF275" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="276" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A276" s="6">
         <v>2026</v>
       </c>
@@ -33956,8 +34829,11 @@
       <c r="AE276" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF276" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="277" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A277" s="6">
         <v>2026</v>
       </c>
@@ -34051,8 +34927,11 @@
       <c r="AE277" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF277" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="278" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A278" s="6">
         <v>2026</v>
       </c>
@@ -34146,8 +35025,11 @@
       <c r="AE278" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF278" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="279" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A279" s="6">
         <v>2026</v>
       </c>
@@ -34241,8 +35123,11 @@
       <c r="AE279" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF279" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="280" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A280" s="6">
         <v>2026</v>
       </c>
@@ -34336,8 +35221,11 @@
       <c r="AE280" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF280" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="281" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A281" s="6">
         <v>2026</v>
       </c>
@@ -34431,8 +35319,11 @@
       <c r="AE281" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF281" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="282" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A282" s="6">
         <v>2026</v>
       </c>
@@ -34526,8 +35417,11 @@
       <c r="AE282" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF282" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="283" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A283" s="6">
         <v>2026</v>
       </c>
@@ -34621,8 +35515,11 @@
       <c r="AE283" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF283" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="284" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A284" s="6">
         <v>2026</v>
       </c>
@@ -34716,8 +35613,11 @@
       <c r="AE284" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF284" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="285" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A285" s="6">
         <v>2026</v>
       </c>
@@ -34811,8 +35711,11 @@
       <c r="AE285" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF285" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="286" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A286" s="6">
         <v>2026</v>
       </c>
@@ -34906,8 +35809,11 @@
       <c r="AE286" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF286" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="287" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A287" s="6">
         <v>2026</v>
       </c>
@@ -35001,8 +35907,11 @@
       <c r="AE287" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF287" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="288" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A288" s="6">
         <v>2026</v>
       </c>
@@ -35096,8 +36005,11 @@
       <c r="AE288" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF288" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="289" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A289" s="6">
         <v>2026</v>
       </c>
@@ -35191,8 +36103,11 @@
       <c r="AE289" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF289" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="290" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A290" s="6">
         <v>2026</v>
       </c>
@@ -35286,8 +36201,11 @@
       <c r="AE290" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF290" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="291" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A291" s="6">
         <v>2026</v>
       </c>
@@ -35381,8 +36299,11 @@
       <c r="AE291" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF291" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="292" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A292" s="6">
         <v>2026</v>
       </c>
@@ -35476,8 +36397,11 @@
       <c r="AE292" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="AF292" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="293" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A293" s="6">
         <v>2026</v>
       </c>
@@ -35571,8 +36495,11 @@
       <c r="AE293" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF293" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="294" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A294" s="6">
         <v>2026</v>
       </c>
@@ -35666,8 +36593,11 @@
       <c r="AE294" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF294" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="295" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A295" s="6">
         <v>2026</v>
       </c>
@@ -35761,8 +36691,11 @@
       <c r="AE295" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF295" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="296" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A296" s="6">
         <v>2026</v>
       </c>
@@ -35856,8 +36789,11 @@
       <c r="AE296" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF296" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="297" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A297" s="6">
         <v>2026</v>
       </c>
@@ -35951,8 +36887,11 @@
       <c r="AE297" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF297" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="298" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A298" s="6">
         <v>2026</v>
       </c>
@@ -36046,8 +36985,11 @@
       <c r="AE298" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF298" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="299" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A299" s="6">
         <v>2026</v>
       </c>
@@ -36141,8 +37083,11 @@
       <c r="AE299" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF299" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="300" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A300" s="6">
         <v>2026</v>
       </c>
@@ -36236,8 +37181,11 @@
       <c r="AE300" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF300" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="301" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A301" s="6">
         <v>2026</v>
       </c>
@@ -36331,8 +37279,11 @@
       <c r="AE301" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF301" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="302" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A302" s="6">
         <v>2026</v>
       </c>
@@ -36426,8 +37377,11 @@
       <c r="AE302" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF302" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="303" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A303" s="6">
         <v>2026</v>
       </c>
@@ -36521,8 +37475,11 @@
       <c r="AE303" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF303" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="304" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A304" s="6">
         <v>2026</v>
       </c>
@@ -36616,8 +37573,11 @@
       <c r="AE304" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF304" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="305" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A305" s="6">
         <v>2026</v>
       </c>
@@ -36711,8 +37671,11 @@
       <c r="AE305" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF305" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="306" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A306" s="6">
         <v>2026</v>
       </c>
@@ -36806,8 +37769,11 @@
       <c r="AE306" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF306" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="307" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A307" s="6">
         <v>2026</v>
       </c>
@@ -36901,8 +37867,11 @@
       <c r="AE307" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF307" s="14" t="s">
+        <v>2419</v>
+      </c>
     </row>
-    <row r="308" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A308" s="6">
         <v>2026</v>
       </c>
@@ -36996,8 +37965,11 @@
       <c r="AE308" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF308" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
-    <row r="309" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A309" s="6">
         <v>2026</v>
       </c>
@@ -37091,8 +38063,11 @@
       <c r="AE309" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF309" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="310" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A310" s="6">
         <v>2026</v>
       </c>
@@ -37186,8 +38161,11 @@
       <c r="AE310" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF310" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="311" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A311" s="6">
         <v>2026</v>
       </c>
@@ -37281,8 +38259,11 @@
       <c r="AE311" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF311" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="312" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A312" s="6">
         <v>2026</v>
       </c>
@@ -37376,8 +38357,11 @@
       <c r="AE312" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF312" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="313" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A313" s="6">
         <v>2026</v>
       </c>
@@ -37471,8 +38455,11 @@
       <c r="AE313" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AF313" s="14" t="s">
+        <v>2418</v>
+      </c>
     </row>
-    <row r="314" spans="1:31" ht="15" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A314" s="6">
         <v>2026</v>
       </c>
@@ -37565,6 +38552,9 @@
       </c>
       <c r="AE314" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="AF314" s="14" t="s">
+        <v>2419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: EXCEL CON REL
</commit_message>
<xml_diff>
--- a/data/propuestas_artisticas.xlsx
+++ b/data/propuestas_artisticas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7744" uniqueCount="2423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7744" uniqueCount="2424">
   <si>
     <t>Edad</t>
   </si>
@@ -7296,6 +7296,9 @@
   </si>
   <si>
     <t>SON_DE_NEGRO</t>
+  </si>
+  <si>
+    <t>DANZAS_REL</t>
   </si>
 </sst>
 </file>
@@ -7775,10 +7778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AF314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AD241" sqref="AD241"/>
+    <sheetView tabSelected="1" topLeftCell="P3" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:AF70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7980,7 +7984,7 @@
         <v>49</v>
       </c>
       <c r="AF2" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -8078,10 +8082,10 @@
         <v>49</v>
       </c>
       <c r="AF3" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2026</v>
       </c>
@@ -8179,7 +8183,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>2026</v>
       </c>
@@ -8277,7 +8281,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>2026</v>
       </c>
@@ -8375,7 +8379,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>2026</v>
       </c>
@@ -8473,7 +8477,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>2026</v>
       </c>
@@ -8666,10 +8670,10 @@
         <v>493</v>
       </c>
       <c r="AF9" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>2026</v>
       </c>
@@ -8862,10 +8866,10 @@
         <v>493</v>
       </c>
       <c r="AF11" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>2026</v>
       </c>
@@ -8963,7 +8967,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>2026</v>
       </c>
@@ -9156,10 +9160,10 @@
         <v>49</v>
       </c>
       <c r="AF14" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>2026</v>
       </c>
@@ -9257,7 +9261,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>2026</v>
       </c>
@@ -9355,7 +9359,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>2026</v>
       </c>
@@ -9453,7 +9457,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>2026</v>
       </c>
@@ -9551,7 +9555,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>2026</v>
       </c>
@@ -9649,7 +9653,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>2026</v>
       </c>
@@ -9842,10 +9846,10 @@
         <v>49</v>
       </c>
       <c r="AF21" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>2026</v>
       </c>
@@ -10038,10 +10042,10 @@
         <v>49</v>
       </c>
       <c r="AF23" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>2026</v>
       </c>
@@ -10234,10 +10238,10 @@
         <v>49</v>
       </c>
       <c r="AF25" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>2026</v>
       </c>
@@ -10335,7 +10339,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>2026</v>
       </c>
@@ -10528,7 +10532,7 @@
         <v>49</v>
       </c>
       <c r="AF28" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -10626,7 +10630,7 @@
         <v>49</v>
       </c>
       <c r="AF29" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -10724,7 +10728,7 @@
         <v>49</v>
       </c>
       <c r="AF30" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="31" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -10822,10 +10826,10 @@
         <v>49</v>
       </c>
       <c r="AF31" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="32" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>2026</v>
       </c>
@@ -10923,7 +10927,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>2026</v>
       </c>
@@ -11116,10 +11120,10 @@
         <v>493</v>
       </c>
       <c r="AF34" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>2026</v>
       </c>
@@ -11217,7 +11221,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="36" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>2026</v>
       </c>
@@ -11315,7 +11319,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="37" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>2026</v>
       </c>
@@ -11413,7 +11417,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="38" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>2026</v>
       </c>
@@ -11511,7 +11515,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="39" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>2026</v>
       </c>
@@ -11704,7 +11708,7 @@
         <v>49</v>
       </c>
       <c r="AF40" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -11802,7 +11806,7 @@
         <v>49</v>
       </c>
       <c r="AF41" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="42" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -11900,7 +11904,7 @@
         <v>49</v>
       </c>
       <c r="AF42" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -11998,10 +12002,10 @@
         <v>493</v>
       </c>
       <c r="AF43" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="44" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>2026</v>
       </c>
@@ -12194,10 +12198,10 @@
         <v>493</v>
       </c>
       <c r="AF45" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>2026</v>
       </c>
@@ -12390,10 +12394,10 @@
         <v>493</v>
       </c>
       <c r="AF47" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="48" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>2026</v>
       </c>
@@ -12586,10 +12590,10 @@
         <v>493</v>
       </c>
       <c r="AF49" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="50" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>2026</v>
       </c>
@@ -12687,7 +12691,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="51" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>2026</v>
       </c>
@@ -12785,7 +12789,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="52" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>2026</v>
       </c>
@@ -12883,7 +12887,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="53" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>2026</v>
       </c>
@@ -12981,7 +12985,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="54" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>2026</v>
       </c>
@@ -13079,7 +13083,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="55" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>2026</v>
       </c>
@@ -13272,10 +13276,10 @@
         <v>493</v>
       </c>
       <c r="AF56" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="57" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>2026</v>
       </c>
@@ -13468,10 +13472,10 @@
         <v>493</v>
       </c>
       <c r="AF58" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="59" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>2026</v>
       </c>
@@ -13664,10 +13668,10 @@
         <v>493</v>
       </c>
       <c r="AF60" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="61" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>2026</v>
       </c>
@@ -13860,10 +13864,10 @@
         <v>49</v>
       </c>
       <c r="AF62" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="63" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>2026</v>
       </c>
@@ -13961,7 +13965,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="64" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>2026</v>
       </c>
@@ -14154,10 +14158,10 @@
         <v>493</v>
       </c>
       <c r="AF65" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="66" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>2026</v>
       </c>
@@ -14255,7 +14259,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="67" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>2026</v>
       </c>
@@ -14448,7 +14452,7 @@
         <v>493</v>
       </c>
       <c r="AF68" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="69" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -14546,7 +14550,7 @@
         <v>493</v>
       </c>
       <c r="AF69" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="70" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -14644,10 +14648,10 @@
         <v>493</v>
       </c>
       <c r="AF70" s="14" t="s">
-        <v>2421</v>
+        <v>2423</v>
       </c>
     </row>
-    <row r="71" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
         <v>2026</v>
       </c>
@@ -14745,7 +14749,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="72" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
         <v>2026</v>
       </c>
@@ -14843,7 +14847,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="73" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
         <v>2026</v>
       </c>
@@ -14941,7 +14945,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="74" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
         <v>2026</v>
       </c>
@@ -15039,7 +15043,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="75" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
         <v>2026</v>
       </c>
@@ -15137,7 +15141,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="76" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
         <v>2026</v>
       </c>
@@ -15235,7 +15239,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="77" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
         <v>2026</v>
       </c>
@@ -15333,7 +15337,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="78" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
         <v>2026</v>
       </c>
@@ -15431,7 +15435,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="79" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
         <v>2026</v>
       </c>
@@ -15529,7 +15533,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="80" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
         <v>2026</v>
       </c>
@@ -15627,7 +15631,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="81" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
         <v>2026</v>
       </c>
@@ -15725,7 +15729,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="82" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
         <v>2026</v>
       </c>
@@ -15823,7 +15827,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="83" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
         <v>2026</v>
       </c>
@@ -15921,7 +15925,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="84" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
         <v>2026</v>
       </c>
@@ -16019,7 +16023,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="85" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
         <v>2026</v>
       </c>
@@ -16117,7 +16121,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="86" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
         <v>2026</v>
       </c>
@@ -16215,7 +16219,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="87" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
         <v>2026</v>
       </c>
@@ -16313,7 +16317,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="88" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
         <v>2026</v>
       </c>
@@ -16411,7 +16415,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="89" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
         <v>2026</v>
       </c>
@@ -16509,7 +16513,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="90" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
         <v>2026</v>
       </c>
@@ -16607,7 +16611,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="91" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
         <v>2026</v>
       </c>
@@ -16705,7 +16709,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="92" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
         <v>2026</v>
       </c>
@@ -16803,7 +16807,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="93" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
         <v>2026</v>
       </c>
@@ -16901,7 +16905,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="94" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
         <v>2026</v>
       </c>
@@ -16999,7 +17003,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="95" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
         <v>2026</v>
       </c>
@@ -17097,7 +17101,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="96" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
         <v>2026</v>
       </c>
@@ -17195,7 +17199,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="97" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
         <v>2026</v>
       </c>
@@ -17293,7 +17297,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="98" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
         <v>2026</v>
       </c>
@@ -17391,7 +17395,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="99" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
         <v>2026</v>
       </c>
@@ -17489,7 +17493,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="100" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
         <v>2026</v>
       </c>
@@ -17587,7 +17591,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="101" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
         <v>2026</v>
       </c>
@@ -17685,7 +17689,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="102" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
         <v>2026</v>
       </c>
@@ -17783,7 +17787,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="103" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
         <v>2026</v>
       </c>
@@ -17881,7 +17885,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="104" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
         <v>2026</v>
       </c>
@@ -17979,7 +17983,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="105" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
         <v>2026</v>
       </c>
@@ -18077,7 +18081,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="106" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
         <v>2026</v>
       </c>
@@ -18175,7 +18179,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="107" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
         <v>2026</v>
       </c>
@@ -18273,7 +18277,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="108" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
         <v>2026</v>
       </c>
@@ -18371,7 +18375,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="109" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="6">
         <v>2026</v>
       </c>
@@ -18469,7 +18473,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="110" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="6">
         <v>2026</v>
       </c>
@@ -18567,7 +18571,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="111" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="6">
         <v>2026</v>
       </c>
@@ -18665,7 +18669,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="112" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="6">
         <v>2026</v>
       </c>
@@ -18763,7 +18767,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="113" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="6">
         <v>2026</v>
       </c>
@@ -18861,7 +18865,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="114" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="6">
         <v>2026</v>
       </c>
@@ -18959,7 +18963,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="115" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="6">
         <v>2026</v>
       </c>
@@ -19057,7 +19061,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="116" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="6">
         <v>2026</v>
       </c>
@@ -19155,7 +19159,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="117" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="6">
         <v>2026</v>
       </c>
@@ -19253,7 +19257,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="118" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="6">
         <v>2026</v>
       </c>
@@ -19351,7 +19355,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="119" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="6">
         <v>2026</v>
       </c>
@@ -19449,7 +19453,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="120" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="6">
         <v>2026</v>
       </c>
@@ -19547,7 +19551,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="121" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="6">
         <v>2026</v>
       </c>
@@ -19645,7 +19649,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="122" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="6">
         <v>2026</v>
       </c>
@@ -19743,7 +19747,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="123" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="6">
         <v>2026</v>
       </c>
@@ -19841,7 +19845,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="124" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="6">
         <v>2026</v>
       </c>
@@ -19939,7 +19943,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="125" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="6">
         <v>2026</v>
       </c>
@@ -20037,7 +20041,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="126" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="6">
         <v>2026</v>
       </c>
@@ -20135,7 +20139,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="127" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="6">
         <v>2026</v>
       </c>
@@ -20233,7 +20237,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="128" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="6">
         <v>2026</v>
       </c>
@@ -20331,7 +20335,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="129" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="6">
         <v>2026</v>
       </c>
@@ -20429,7 +20433,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="130" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="6">
         <v>2026</v>
       </c>
@@ -20527,7 +20531,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="131" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="6">
         <v>2026</v>
       </c>
@@ -20625,7 +20629,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="132" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="6">
         <v>2026</v>
       </c>
@@ -20723,7 +20727,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="133" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="6">
         <v>2026</v>
       </c>
@@ -20821,7 +20825,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="134" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="6">
         <v>2026</v>
       </c>
@@ -20919,7 +20923,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="135" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="6">
         <v>2026</v>
       </c>
@@ -21017,7 +21021,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="136" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="6">
         <v>2026</v>
       </c>
@@ -21115,7 +21119,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="137" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="6">
         <v>2026</v>
       </c>
@@ -21213,7 +21217,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="138" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="6">
         <v>2026</v>
       </c>
@@ -21311,7 +21315,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="139" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="6">
         <v>2026</v>
       </c>
@@ -21409,7 +21413,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="140" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="6">
         <v>2026</v>
       </c>
@@ -21507,7 +21511,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="141" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
         <v>2026</v>
       </c>
@@ -21605,7 +21609,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="142" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="6">
         <v>2026</v>
       </c>
@@ -21703,7 +21707,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="143" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="6">
         <v>2026</v>
       </c>
@@ -21801,7 +21805,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="144" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="6">
         <v>2026</v>
       </c>
@@ -21899,7 +21903,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="145" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="6">
         <v>2026</v>
       </c>
@@ -21997,7 +22001,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="146" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="6">
         <v>2026</v>
       </c>
@@ -22095,7 +22099,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="147" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="6">
         <v>2026</v>
       </c>
@@ -22193,7 +22197,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="148" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="6">
         <v>2026</v>
       </c>
@@ -22291,7 +22295,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="149" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="6">
         <v>2026</v>
       </c>
@@ -22389,7 +22393,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="150" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="6">
         <v>2026</v>
       </c>
@@ -22487,7 +22491,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="151" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="6">
         <v>2026</v>
       </c>
@@ -22585,7 +22589,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="152" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="6">
         <v>2026</v>
       </c>
@@ -22683,7 +22687,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="153" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="6">
         <v>2026</v>
       </c>
@@ -22781,7 +22785,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="154" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="6">
         <v>2026</v>
       </c>
@@ -22879,7 +22883,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="155" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="6">
         <v>2026</v>
       </c>
@@ -22977,7 +22981,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="156" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" s="6">
         <v>2026</v>
       </c>
@@ -23075,7 +23079,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="157" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" s="6">
         <v>2026</v>
       </c>
@@ -23173,7 +23177,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="158" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="6">
         <v>2026</v>
       </c>
@@ -23271,7 +23275,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="159" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="6">
         <v>2026</v>
       </c>
@@ -23369,7 +23373,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="160" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="6">
         <v>2026</v>
       </c>
@@ -23467,7 +23471,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="161" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="6">
         <v>2026</v>
       </c>
@@ -23565,7 +23569,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="162" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" s="6">
         <v>2026</v>
       </c>
@@ -23663,7 +23667,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="163" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="6">
         <v>2026</v>
       </c>
@@ -23761,7 +23765,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="164" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="6">
         <v>2026</v>
       </c>
@@ -23859,7 +23863,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="165" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="6">
         <v>2026</v>
       </c>
@@ -23957,7 +23961,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="166" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="6">
         <v>2026</v>
       </c>
@@ -24055,7 +24059,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="167" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" s="6">
         <v>2026</v>
       </c>
@@ -24153,7 +24157,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="168" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="6">
         <v>2026</v>
       </c>
@@ -24251,7 +24255,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="169" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="6">
         <v>2026</v>
       </c>
@@ -24349,7 +24353,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="170" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="6">
         <v>2026</v>
       </c>
@@ -24447,7 +24451,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="171" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="6">
         <v>2026</v>
       </c>
@@ -24545,7 +24549,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="172" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="6">
         <v>2026</v>
       </c>
@@ -24643,7 +24647,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="173" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" s="6">
         <v>2026</v>
       </c>
@@ -24741,7 +24745,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="174" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="6">
         <v>2026</v>
       </c>
@@ -24839,7 +24843,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="175" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" s="6">
         <v>2026</v>
       </c>
@@ -24937,7 +24941,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="176" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="6">
         <v>2026</v>
       </c>
@@ -25035,7 +25039,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="177" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="6">
         <v>2026</v>
       </c>
@@ -25133,7 +25137,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="178" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="6">
         <v>2026</v>
       </c>
@@ -25231,7 +25235,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="179" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="6">
         <v>2026</v>
       </c>
@@ -25329,7 +25333,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="180" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="6">
         <v>2026</v>
       </c>
@@ -25427,7 +25431,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="181" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="6">
         <v>2026</v>
       </c>
@@ -25525,7 +25529,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="182" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="9">
         <v>2026</v>
       </c>
@@ -25623,7 +25627,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="183" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="6">
         <v>2026</v>
       </c>
@@ -25721,7 +25725,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="184" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="6">
         <v>2026</v>
       </c>
@@ -25819,7 +25823,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="185" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="6">
         <v>2026</v>
       </c>
@@ -25917,7 +25921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="6">
         <v>2026</v>
       </c>
@@ -26015,7 +26019,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="187" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="6">
         <v>2026</v>
       </c>
@@ -26113,7 +26117,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="6">
         <v>2026</v>
       </c>
@@ -26211,7 +26215,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="189" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="6">
         <v>2026</v>
       </c>
@@ -26309,7 +26313,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="190" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="6">
         <v>2026</v>
       </c>
@@ -26407,7 +26411,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="6">
         <v>2026</v>
       </c>
@@ -26505,7 +26509,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="192" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" s="6">
         <v>2026</v>
       </c>
@@ -26603,7 +26607,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="193" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="6">
         <v>2026</v>
       </c>
@@ -26701,7 +26705,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="194" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" s="6">
         <v>2026</v>
       </c>
@@ -26799,7 +26803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="6">
         <v>2026</v>
       </c>
@@ -26897,7 +26901,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="196" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" s="6">
         <v>2026</v>
       </c>
@@ -26995,7 +26999,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="197" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" s="6">
         <v>2026</v>
       </c>
@@ -27093,7 +27097,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="198" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" s="6">
         <v>2026</v>
       </c>
@@ -27191,7 +27195,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="199" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" s="6">
         <v>2026</v>
       </c>
@@ -27289,7 +27293,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="200" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" s="6">
         <v>2026</v>
       </c>
@@ -27387,7 +27391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="201" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" s="6">
         <v>2026</v>
       </c>
@@ -27485,7 +27489,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="202" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="6">
         <v>2026</v>
       </c>
@@ -27583,7 +27587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="6">
         <v>2026</v>
       </c>
@@ -27681,7 +27685,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="204" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="6">
         <v>2026</v>
       </c>
@@ -27779,7 +27783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="205" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="6">
         <v>2026</v>
       </c>
@@ -27877,7 +27881,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="206" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="6">
         <v>2026</v>
       </c>
@@ -27975,7 +27979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="207" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="6">
         <v>2026</v>
       </c>
@@ -28073,7 +28077,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="6">
         <v>2026</v>
       </c>
@@ -28171,7 +28175,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="209" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="6">
         <v>2026</v>
       </c>
@@ -28269,7 +28273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="210" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="6">
         <v>2026</v>
       </c>
@@ -28367,7 +28371,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="211" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="6">
         <v>2026</v>
       </c>
@@ -28465,7 +28469,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="6">
         <v>2026</v>
       </c>
@@ -28563,7 +28567,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="213" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="6">
         <v>2026</v>
       </c>
@@ -28661,7 +28665,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="214" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="6">
         <v>2026</v>
       </c>
@@ -28759,7 +28763,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="215" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="6">
         <v>2026</v>
       </c>
@@ -28857,7 +28861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="216" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="6">
         <v>2026</v>
       </c>
@@ -28955,7 +28959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="217" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="6">
         <v>2026</v>
       </c>
@@ -29053,7 +29057,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="218" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="6">
         <v>2026</v>
       </c>
@@ -29151,7 +29155,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="219" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="6">
         <v>2026</v>
       </c>
@@ -29249,7 +29253,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="220" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="6">
         <v>2026</v>
       </c>
@@ -29347,7 +29351,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="221" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" s="6">
         <v>2026</v>
       </c>
@@ -29445,7 +29449,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="222" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" s="6">
         <v>2026</v>
       </c>
@@ -29543,7 +29547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="223" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" s="6">
         <v>2026</v>
       </c>
@@ -29641,7 +29645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" s="6">
         <v>2026</v>
       </c>
@@ -29739,7 +29743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="225" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" s="6">
         <v>2026</v>
       </c>
@@ -29837,7 +29841,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="226" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" s="6">
         <v>2026</v>
       </c>
@@ -29935,7 +29939,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="227" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" s="6">
         <v>2026</v>
       </c>
@@ -30033,7 +30037,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" s="6">
         <v>2026</v>
       </c>
@@ -30131,7 +30135,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="229" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" s="6">
         <v>2026</v>
       </c>
@@ -30229,7 +30233,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="230" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" s="6">
         <v>2026</v>
       </c>
@@ -30327,7 +30331,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="231" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" s="6">
         <v>2026</v>
       </c>
@@ -30425,7 +30429,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="232" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" s="6">
         <v>2026</v>
       </c>
@@ -30523,7 +30527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="233" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" s="6">
         <v>2026</v>
       </c>
@@ -30621,7 +30625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="234" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" s="6">
         <v>2026</v>
       </c>
@@ -30719,7 +30723,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="235" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" s="6">
         <v>2026</v>
       </c>
@@ -30817,7 +30821,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="236" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" s="6">
         <v>2026</v>
       </c>
@@ -30915,7 +30919,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="237" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" s="6">
         <v>2026</v>
       </c>
@@ -31013,7 +31017,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="238" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" s="6">
         <v>2026</v>
       </c>
@@ -31111,7 +31115,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="239" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" s="6">
         <v>2026</v>
       </c>
@@ -31209,7 +31213,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="240" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" s="6">
         <v>2026</v>
       </c>
@@ -31307,7 +31311,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="241" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" s="6">
         <v>2026</v>
       </c>
@@ -31405,7 +31409,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="242" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" s="6">
         <v>2026</v>
       </c>
@@ -31503,7 +31507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="243" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" s="6">
         <v>2026</v>
       </c>
@@ -31601,7 +31605,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="244" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" s="6">
         <v>2026</v>
       </c>
@@ -31699,7 +31703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="245" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245" s="6">
         <v>2026</v>
       </c>
@@ -31797,7 +31801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="246" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246" s="6">
         <v>2026</v>
       </c>
@@ -31895,7 +31899,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="247" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" s="6">
         <v>2026</v>
       </c>
@@ -31993,7 +31997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="248" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" s="6">
         <v>2026</v>
       </c>
@@ -32091,7 +32095,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="249" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" s="6">
         <v>2026</v>
       </c>
@@ -32189,7 +32193,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="250" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" s="6">
         <v>2026</v>
       </c>
@@ -32287,7 +32291,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="251" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" s="6">
         <v>2026</v>
       </c>
@@ -32383,7 +32387,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="252" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" s="6">
         <v>2026</v>
       </c>
@@ -32481,7 +32485,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="253" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253" s="6">
         <v>2026</v>
       </c>
@@ -32579,7 +32583,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="254" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254" s="6">
         <v>2026</v>
       </c>
@@ -32677,7 +32681,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="255" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" s="6">
         <v>2026</v>
       </c>
@@ -32775,7 +32779,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="256" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256" s="6">
         <v>2026</v>
       </c>
@@ -32873,7 +32877,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="257" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257" s="6">
         <v>2026</v>
       </c>
@@ -32971,7 +32975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="258" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258" s="6">
         <v>2026</v>
       </c>
@@ -33069,7 +33073,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="259" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A259" s="6">
         <v>2026</v>
       </c>
@@ -33167,7 +33171,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="260" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" s="6">
         <v>2026</v>
       </c>
@@ -33265,7 +33269,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="261" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" s="6">
         <v>2026</v>
       </c>
@@ -33363,7 +33367,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="262" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" s="6">
         <v>2026</v>
       </c>
@@ -33461,7 +33465,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="263" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" s="6">
         <v>2026</v>
       </c>
@@ -33559,7 +33563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="264" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" s="6">
         <v>2026</v>
       </c>
@@ -33657,7 +33661,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="265" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" s="6">
         <v>2026</v>
       </c>
@@ -33755,7 +33759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="266" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" s="6">
         <v>2026</v>
       </c>
@@ -33853,7 +33857,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="267" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" s="6">
         <v>2026</v>
       </c>
@@ -33951,7 +33955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="268" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268" s="6">
         <v>2026</v>
       </c>
@@ -34049,7 +34053,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="269" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" s="6">
         <v>2026</v>
       </c>
@@ -34147,7 +34151,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="270" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" s="6">
         <v>2026</v>
       </c>
@@ -34245,7 +34249,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="271" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271" s="6">
         <v>2026</v>
       </c>
@@ -34343,7 +34347,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="272" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" s="6">
         <v>2026</v>
       </c>
@@ -34441,7 +34445,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="273" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" s="6">
         <v>2026</v>
       </c>
@@ -34539,7 +34543,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="274" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" s="6">
         <v>2026</v>
       </c>
@@ -34637,7 +34641,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="275" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" s="6">
         <v>2026</v>
       </c>
@@ -34735,7 +34739,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="276" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" s="6">
         <v>2026</v>
       </c>
@@ -34833,7 +34837,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="277" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" s="6">
         <v>2026</v>
       </c>
@@ -34931,7 +34935,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="278" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" s="6">
         <v>2026</v>
       </c>
@@ -35029,7 +35033,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="279" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279" s="6">
         <v>2026</v>
       </c>
@@ -35127,7 +35131,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="280" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280" s="6">
         <v>2026</v>
       </c>
@@ -35225,7 +35229,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="281" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" s="6">
         <v>2026</v>
       </c>
@@ -35323,7 +35327,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="282" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A282" s="6">
         <v>2026</v>
       </c>
@@ -35421,7 +35425,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="283" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283" s="6">
         <v>2026</v>
       </c>
@@ -35519,7 +35523,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="284" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284" s="6">
         <v>2026</v>
       </c>
@@ -35617,7 +35621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="285" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A285" s="6">
         <v>2026</v>
       </c>
@@ -35715,7 +35719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="286" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A286" s="6">
         <v>2026</v>
       </c>
@@ -35813,7 +35817,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="287" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A287" s="6">
         <v>2026</v>
       </c>
@@ -35911,7 +35915,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="288" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A288" s="6">
         <v>2026</v>
       </c>
@@ -36009,7 +36013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="289" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289" s="6">
         <v>2026</v>
       </c>
@@ -36107,7 +36111,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="290" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290" s="6">
         <v>2026</v>
       </c>
@@ -36205,7 +36209,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="291" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291" s="6">
         <v>2026</v>
       </c>
@@ -36303,7 +36307,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="292" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292" s="6">
         <v>2026</v>
       </c>
@@ -36401,7 +36405,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="293" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A293" s="6">
         <v>2026</v>
       </c>
@@ -36499,7 +36503,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="294" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" s="6">
         <v>2026</v>
       </c>
@@ -36597,7 +36601,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="295" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A295" s="6">
         <v>2026</v>
       </c>
@@ -36695,7 +36699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="296" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A296" s="6">
         <v>2026</v>
       </c>
@@ -36793,7 +36797,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="297" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A297" s="6">
         <v>2026</v>
       </c>
@@ -36891,7 +36895,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="298" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A298" s="6">
         <v>2026</v>
       </c>
@@ -36989,7 +36993,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="299" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A299" s="6">
         <v>2026</v>
       </c>
@@ -37087,7 +37091,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="300" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A300" s="6">
         <v>2026</v>
       </c>
@@ -37185,7 +37189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="301" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A301" s="6">
         <v>2026</v>
       </c>
@@ -37283,7 +37287,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="302" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A302" s="6">
         <v>2026</v>
       </c>
@@ -37381,7 +37385,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="303" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A303" s="6">
         <v>2026</v>
       </c>
@@ -37479,7 +37483,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="304" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A304" s="6">
         <v>2026</v>
       </c>
@@ -37577,7 +37581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="305" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A305" s="6">
         <v>2026</v>
       </c>
@@ -37675,7 +37679,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="306" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A306" s="6">
         <v>2026</v>
       </c>
@@ -37773,7 +37777,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="307" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A307" s="6">
         <v>2026</v>
       </c>
@@ -37871,7 +37875,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="308" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A308" s="6">
         <v>2026</v>
       </c>
@@ -37969,7 +37973,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="309" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A309" s="6">
         <v>2026</v>
       </c>
@@ -38067,7 +38071,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="310" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A310" s="6">
         <v>2026</v>
       </c>
@@ -38165,7 +38169,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="311" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A311" s="6">
         <v>2026</v>
       </c>
@@ -38263,7 +38267,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="312" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A312" s="6">
         <v>2026</v>
       </c>
@@ -38361,7 +38365,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="313" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A313" s="6">
         <v>2026</v>
       </c>
@@ -38459,7 +38463,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="314" spans="1:32" ht="15" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:32" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A314" s="6">
         <v>2026</v>
       </c>
@@ -38559,6 +38563,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AE314">
+    <filterColumn colId="26">
+      <filters>
+        <filter val="DANZA DE RELACIÓN"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:AE314">
       <sortCondition ref="Z1:Z314"/>
     </sortState>

</xml_diff>